<commit_message>
ajuste na base de dados
</commit_message>
<xml_diff>
--- a/base_de_dados/base_dados.xlsx
+++ b/base_de_dados/base_dados.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/b_nascimento_silva_accenture_com/Documents/Desktop/automatizador/base_de_dados/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_81AEDCC69BE12BE590160BCAE35EEE27512C17AC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{688F93D4-A6A1-4710-A486-E71495ABF731}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -421,306 +427,6 @@
     <t>Aragão</t>
   </si>
   <si>
-    <t>29/11/1982</t>
-  </si>
-  <si>
-    <t>02/07/1985</t>
-  </si>
-  <si>
-    <t>14/10/1987</t>
-  </si>
-  <si>
-    <t>13/04/1979</t>
-  </si>
-  <si>
-    <t>01/07/1979</t>
-  </si>
-  <si>
-    <t>25/02/1997</t>
-  </si>
-  <si>
-    <t>02/08/1974</t>
-  </si>
-  <si>
-    <t>07/03/1985</t>
-  </si>
-  <si>
-    <t>29/07/1970</t>
-  </si>
-  <si>
-    <t>04/04/1968</t>
-  </si>
-  <si>
-    <t>03/07/1975</t>
-  </si>
-  <si>
-    <t>28/08/2000</t>
-  </si>
-  <si>
-    <t>21/05/2006</t>
-  </si>
-  <si>
-    <t>05/05/1978</t>
-  </si>
-  <si>
-    <t>05/03/1996</t>
-  </si>
-  <si>
-    <t>19/05/1973</t>
-  </si>
-  <si>
-    <t>06/07/1977</t>
-  </si>
-  <si>
-    <t>15/01/1980</t>
-  </si>
-  <si>
-    <t>23/04/1990</t>
-  </si>
-  <si>
-    <t>14/01/1972</t>
-  </si>
-  <si>
-    <t>08/10/1984</t>
-  </si>
-  <si>
-    <t>03/12/1984</t>
-  </si>
-  <si>
-    <t>23/03/1995</t>
-  </si>
-  <si>
-    <t>23/09/1959</t>
-  </si>
-  <si>
-    <t>27/02/1997</t>
-  </si>
-  <si>
-    <t>06/08/1984</t>
-  </si>
-  <si>
-    <t>28/07/1999</t>
-  </si>
-  <si>
-    <t>10/04/1983</t>
-  </si>
-  <si>
-    <t>02/10/1987</t>
-  </si>
-  <si>
-    <t>28/07/2002</t>
-  </si>
-  <si>
-    <t>20/07/1995</t>
-  </si>
-  <si>
-    <t>12/10/1982</t>
-  </si>
-  <si>
-    <t>24/08/1987</t>
-  </si>
-  <si>
-    <t>03/11/1993</t>
-  </si>
-  <si>
-    <t>24/07/1999</t>
-  </si>
-  <si>
-    <t>09/12/1969</t>
-  </si>
-  <si>
-    <t>10/09/1988</t>
-  </si>
-  <si>
-    <t>14/06/1994</t>
-  </si>
-  <si>
-    <t>26/06/1962</t>
-  </si>
-  <si>
-    <t>06/12/1967</t>
-  </si>
-  <si>
-    <t>19/12/1997</t>
-  </si>
-  <si>
-    <t>24/06/1996</t>
-  </si>
-  <si>
-    <t>16/12/1975</t>
-  </si>
-  <si>
-    <t>11/08/1997</t>
-  </si>
-  <si>
-    <t>05/06/1995</t>
-  </si>
-  <si>
-    <t>03/02/1987</t>
-  </si>
-  <si>
-    <t>22/01/1988</t>
-  </si>
-  <si>
-    <t>23/06/1993</t>
-  </si>
-  <si>
-    <t>30/06/1986</t>
-  </si>
-  <si>
-    <t>08/09/1967</t>
-  </si>
-  <si>
-    <t>23/10/1966</t>
-  </si>
-  <si>
-    <t>08/06/1995</t>
-  </si>
-  <si>
-    <t>25/02/1961</t>
-  </si>
-  <si>
-    <t>29/02/2000</t>
-  </si>
-  <si>
-    <t>09/09/1960</t>
-  </si>
-  <si>
-    <t>17/06/1978</t>
-  </si>
-  <si>
-    <t>13/09/1985</t>
-  </si>
-  <si>
-    <t>20/07/1967</t>
-  </si>
-  <si>
-    <t>13/02/1998</t>
-  </si>
-  <si>
-    <t>04/05/1993</t>
-  </si>
-  <si>
-    <t>21/03/1984</t>
-  </si>
-  <si>
-    <t>29/08/1978</t>
-  </si>
-  <si>
-    <t>28/05/1995</t>
-  </si>
-  <si>
-    <t>27/02/1962</t>
-  </si>
-  <si>
-    <t>26/10/1964</t>
-  </si>
-  <si>
-    <t>03/05/1965</t>
-  </si>
-  <si>
-    <t>31/10/1997</t>
-  </si>
-  <si>
-    <t>26/04/1971</t>
-  </si>
-  <si>
-    <t>20/02/1977</t>
-  </si>
-  <si>
-    <t>10/10/1976</t>
-  </si>
-  <si>
-    <t>03/07/1969</t>
-  </si>
-  <si>
-    <t>27/12/1993</t>
-  </si>
-  <si>
-    <t>13/01/1972</t>
-  </si>
-  <si>
-    <t>25/09/2002</t>
-  </si>
-  <si>
-    <t>04/12/1998</t>
-  </si>
-  <si>
-    <t>12/07/1967</t>
-  </si>
-  <si>
-    <t>02/10/1965</t>
-  </si>
-  <si>
-    <t>23/08/1998</t>
-  </si>
-  <si>
-    <t>13/03/1979</t>
-  </si>
-  <si>
-    <t>20/01/1968</t>
-  </si>
-  <si>
-    <t>21/07/1994</t>
-  </si>
-  <si>
-    <t>04/02/1969</t>
-  </si>
-  <si>
-    <t>11/04/1968</t>
-  </si>
-  <si>
-    <t>25/03/1982</t>
-  </si>
-  <si>
-    <t>20/09/1978</t>
-  </si>
-  <si>
-    <t>08/05/2002</t>
-  </si>
-  <si>
-    <t>18/10/1969</t>
-  </si>
-  <si>
-    <t>01/04/1985</t>
-  </si>
-  <si>
-    <t>07/02/1961</t>
-  </si>
-  <si>
-    <t>24/04/1964</t>
-  </si>
-  <si>
-    <t>21/11/1998</t>
-  </si>
-  <si>
-    <t>10/07/1987</t>
-  </si>
-  <si>
-    <t>12/07/1969</t>
-  </si>
-  <si>
-    <t>16/07/2001</t>
-  </si>
-  <si>
-    <t>25/06/1972</t>
-  </si>
-  <si>
-    <t>12/09/1983</t>
-  </si>
-  <si>
-    <t>21/11/2003</t>
-  </si>
-  <si>
-    <t>28/01/2004</t>
-  </si>
-  <si>
-    <t>21/08/1997</t>
-  </si>
-  <si>
-    <t>19/05/1982</t>
-  </si>
-  <si>
     <t>Esteticista</t>
   </si>
   <si>
@@ -892,15 +598,9 @@
     <t>Lancheiro</t>
   </si>
   <si>
-    <t>Taxidermista/Embalsamador</t>
-  </si>
-  <si>
     <t>Profissional de logística</t>
   </si>
   <si>
-    <t>Coveiro/Sepultador</t>
-  </si>
-  <si>
     <t>Engenheiro aeronáutico</t>
   </si>
   <si>
@@ -994,17 +694,323 @@
     <t>Artista plástico</t>
   </si>
   <si>
-    <t>Broker/Corretor da bolsa de valores</t>
-  </si>
-  <si>
     <t>Topógrafo</t>
+  </si>
+  <si>
+    <t>29.11.1982</t>
+  </si>
+  <si>
+    <t>02.07.1985</t>
+  </si>
+  <si>
+    <t>14.10.1987</t>
+  </si>
+  <si>
+    <t>13.04.1979</t>
+  </si>
+  <si>
+    <t>01.07.1979</t>
+  </si>
+  <si>
+    <t>25.02.1997</t>
+  </si>
+  <si>
+    <t>02.08.1974</t>
+  </si>
+  <si>
+    <t>07.03.1985</t>
+  </si>
+  <si>
+    <t>29.07.1970</t>
+  </si>
+  <si>
+    <t>04.04.1968</t>
+  </si>
+  <si>
+    <t>03.07.1975</t>
+  </si>
+  <si>
+    <t>28.08.2000</t>
+  </si>
+  <si>
+    <t>21.05.2006</t>
+  </si>
+  <si>
+    <t>05.05.1978</t>
+  </si>
+  <si>
+    <t>05.03.1996</t>
+  </si>
+  <si>
+    <t>19.05.1973</t>
+  </si>
+  <si>
+    <t>06.07.1977</t>
+  </si>
+  <si>
+    <t>15.01.1980</t>
+  </si>
+  <si>
+    <t>23.04.1990</t>
+  </si>
+  <si>
+    <t>14.01.1972</t>
+  </si>
+  <si>
+    <t>08.10.1984</t>
+  </si>
+  <si>
+    <t>03.12.1984</t>
+  </si>
+  <si>
+    <t>23.03.1995</t>
+  </si>
+  <si>
+    <t>23.09.1959</t>
+  </si>
+  <si>
+    <t>27.02.1997</t>
+  </si>
+  <si>
+    <t>06.08.1984</t>
+  </si>
+  <si>
+    <t>28.07.1999</t>
+  </si>
+  <si>
+    <t>10.04.1983</t>
+  </si>
+  <si>
+    <t>02.10.1987</t>
+  </si>
+  <si>
+    <t>28.07.2002</t>
+  </si>
+  <si>
+    <t>20.07.1995</t>
+  </si>
+  <si>
+    <t>12.10.1982</t>
+  </si>
+  <si>
+    <t>24.08.1987</t>
+  </si>
+  <si>
+    <t>03.11.1993</t>
+  </si>
+  <si>
+    <t>24.07.1999</t>
+  </si>
+  <si>
+    <t>09.12.1969</t>
+  </si>
+  <si>
+    <t>10.09.1988</t>
+  </si>
+  <si>
+    <t>14.06.1994</t>
+  </si>
+  <si>
+    <t>26.06.1962</t>
+  </si>
+  <si>
+    <t>06.12.1967</t>
+  </si>
+  <si>
+    <t>19.12.1997</t>
+  </si>
+  <si>
+    <t>24.06.1996</t>
+  </si>
+  <si>
+    <t>16.12.1975</t>
+  </si>
+  <si>
+    <t>11.08.1997</t>
+  </si>
+  <si>
+    <t>05.06.1995</t>
+  </si>
+  <si>
+    <t>03.02.1987</t>
+  </si>
+  <si>
+    <t>22.01.1988</t>
+  </si>
+  <si>
+    <t>23.06.1993</t>
+  </si>
+  <si>
+    <t>30.06.1986</t>
+  </si>
+  <si>
+    <t>08.09.1967</t>
+  </si>
+  <si>
+    <t>23.10.1966</t>
+  </si>
+  <si>
+    <t>08.06.1995</t>
+  </si>
+  <si>
+    <t>25.02.1961</t>
+  </si>
+  <si>
+    <t>29.02.2000</t>
+  </si>
+  <si>
+    <t>09.09.1960</t>
+  </si>
+  <si>
+    <t>17.06.1978</t>
+  </si>
+  <si>
+    <t>13.09.1985</t>
+  </si>
+  <si>
+    <t>20.07.1967</t>
+  </si>
+  <si>
+    <t>13.02.1998</t>
+  </si>
+  <si>
+    <t>04.05.1993</t>
+  </si>
+  <si>
+    <t>Taxidermista.Embalsamador</t>
+  </si>
+  <si>
+    <t>21.03.1984</t>
+  </si>
+  <si>
+    <t>29.08.1978</t>
+  </si>
+  <si>
+    <t>Coveiro.Sepultador</t>
+  </si>
+  <si>
+    <t>28.05.1995</t>
+  </si>
+  <si>
+    <t>27.02.1962</t>
+  </si>
+  <si>
+    <t>26.10.1964</t>
+  </si>
+  <si>
+    <t>03.05.1965</t>
+  </si>
+  <si>
+    <t>31.10.1997</t>
+  </si>
+  <si>
+    <t>26.04.1971</t>
+  </si>
+  <si>
+    <t>20.02.1977</t>
+  </si>
+  <si>
+    <t>10.10.1976</t>
+  </si>
+  <si>
+    <t>03.07.1969</t>
+  </si>
+  <si>
+    <t>27.12.1993</t>
+  </si>
+  <si>
+    <t>13.01.1972</t>
+  </si>
+  <si>
+    <t>25.09.2002</t>
+  </si>
+  <si>
+    <t>04.12.1998</t>
+  </si>
+  <si>
+    <t>12.07.1967</t>
+  </si>
+  <si>
+    <t>02.10.1965</t>
+  </si>
+  <si>
+    <t>23.08.1998</t>
+  </si>
+  <si>
+    <t>13.03.1979</t>
+  </si>
+  <si>
+    <t>20.01.1968</t>
+  </si>
+  <si>
+    <t>21.07.1994</t>
+  </si>
+  <si>
+    <t>04.02.1969</t>
+  </si>
+  <si>
+    <t>11.04.1968</t>
+  </si>
+  <si>
+    <t>25.03.1982</t>
+  </si>
+  <si>
+    <t>20.09.1978</t>
+  </si>
+  <si>
+    <t>08.05.2002</t>
+  </si>
+  <si>
+    <t>18.10.1969</t>
+  </si>
+  <si>
+    <t>01.04.1985</t>
+  </si>
+  <si>
+    <t>07.02.1961</t>
+  </si>
+  <si>
+    <t>24.04.1964</t>
+  </si>
+  <si>
+    <t>21.11.1998</t>
+  </si>
+  <si>
+    <t>10.07.1987</t>
+  </si>
+  <si>
+    <t>12.07.1969</t>
+  </si>
+  <si>
+    <t>16.07.2001</t>
+  </si>
+  <si>
+    <t>25.06.1972</t>
+  </si>
+  <si>
+    <t>12.09.1983</t>
+  </si>
+  <si>
+    <t>21.11.2003</t>
+  </si>
+  <si>
+    <t>28.01.2004</t>
+  </si>
+  <si>
+    <t>21.08.1997</t>
+  </si>
+  <si>
+    <t>Broker.Corretor da bolsa de valores</t>
+  </si>
+  <si>
+    <t>19.05.1982</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1067,13 +1073,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1111,7 +1125,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1145,6 +1159,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1179,9 +1194,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1354,14 +1370,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1375,7 +1393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1383,13 +1401,13 @@
         <v>85</v>
       </c>
       <c r="C2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" t="s">
         <v>135</v>
       </c>
-      <c r="D2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1397,13 +1415,13 @@
         <v>86</v>
       </c>
       <c r="C3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" t="s">
         <v>136</v>
       </c>
-      <c r="D3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1411,13 +1429,13 @@
         <v>87</v>
       </c>
       <c r="C4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" t="s">
         <v>137</v>
       </c>
-      <c r="D4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1425,13 +1443,13 @@
         <v>88</v>
       </c>
       <c r="C5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" t="s">
         <v>138</v>
       </c>
-      <c r="D5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1439,13 +1457,13 @@
         <v>89</v>
       </c>
       <c r="C6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" t="s">
         <v>139</v>
       </c>
-      <c r="D6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1453,13 +1471,13 @@
         <v>88</v>
       </c>
       <c r="C7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" t="s">
         <v>140</v>
       </c>
-      <c r="D7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1467,13 +1485,13 @@
         <v>90</v>
       </c>
       <c r="C8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" t="s">
         <v>141</v>
       </c>
-      <c r="D8" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1481,13 +1499,13 @@
         <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>232</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1495,13 +1513,13 @@
         <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>233</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1509,13 +1527,13 @@
         <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>234</v>
       </c>
       <c r="D11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1523,13 +1541,13 @@
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>235</v>
       </c>
       <c r="D12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1537,13 +1555,13 @@
         <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
       <c r="D13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1551,13 +1569,13 @@
         <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>237</v>
       </c>
       <c r="D14" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1565,13 +1583,13 @@
         <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>238</v>
       </c>
       <c r="D15" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1579,13 +1597,13 @@
         <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>239</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1593,13 +1611,13 @@
         <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>150</v>
+        <v>240</v>
       </c>
       <c r="D17" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1607,13 +1625,13 @@
         <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>151</v>
+        <v>241</v>
       </c>
       <c r="D18" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1621,13 +1639,13 @@
         <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>242</v>
       </c>
       <c r="D19" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1635,13 +1653,13 @@
         <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>243</v>
       </c>
       <c r="D20" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1649,13 +1667,13 @@
         <v>101</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>244</v>
       </c>
       <c r="D21" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1663,13 +1681,13 @@
         <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>245</v>
       </c>
       <c r="D22" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1677,13 +1695,13 @@
         <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>246</v>
       </c>
       <c r="D23" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1691,13 +1709,13 @@
         <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>157</v>
+        <v>247</v>
       </c>
       <c r="D24" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1705,13 +1723,13 @@
         <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>158</v>
+        <v>248</v>
       </c>
       <c r="D25" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1719,13 +1737,13 @@
         <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c r="D26" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1733,13 +1751,13 @@
         <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="D27" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1747,13 +1765,13 @@
         <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>161</v>
+        <v>251</v>
       </c>
       <c r="D28" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1761,13 +1779,13 @@
         <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>252</v>
       </c>
       <c r="D29" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1775,13 +1793,13 @@
         <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>253</v>
       </c>
       <c r="D30" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1789,13 +1807,13 @@
         <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>164</v>
+        <v>254</v>
       </c>
       <c r="D31" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1803,13 +1821,13 @@
         <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>255</v>
       </c>
       <c r="D32" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1817,13 +1835,13 @@
         <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>166</v>
+        <v>256</v>
       </c>
       <c r="D33" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1831,13 +1849,13 @@
         <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>257</v>
       </c>
       <c r="D34" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1845,13 +1863,13 @@
         <v>110</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>258</v>
       </c>
       <c r="D35" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1859,13 +1877,13 @@
         <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>169</v>
+        <v>259</v>
       </c>
       <c r="D36" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1873,13 +1891,13 @@
         <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>170</v>
+        <v>260</v>
       </c>
       <c r="D37" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1887,13 +1905,13 @@
         <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>171</v>
+        <v>261</v>
       </c>
       <c r="D38" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1901,13 +1919,13 @@
         <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>172</v>
+        <v>262</v>
       </c>
       <c r="D39" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1915,13 +1933,13 @@
         <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="D40" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1929,13 +1947,13 @@
         <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="D41" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1943,13 +1961,13 @@
         <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>175</v>
+        <v>265</v>
       </c>
       <c r="D42" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1957,13 +1975,13 @@
         <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>176</v>
+        <v>266</v>
       </c>
       <c r="D43" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1971,13 +1989,13 @@
         <v>115</v>
       </c>
       <c r="C44" t="s">
-        <v>177</v>
+        <v>267</v>
       </c>
       <c r="D44" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1985,13 +2003,13 @@
         <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>178</v>
+        <v>268</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1999,13 +2017,13 @@
         <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>179</v>
+        <v>269</v>
       </c>
       <c r="D46" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -2013,13 +2031,13 @@
         <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="D47" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -2027,13 +2045,13 @@
         <v>103</v>
       </c>
       <c r="C48" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
       <c r="D48" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -2041,13 +2059,13 @@
         <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>182</v>
+        <v>272</v>
       </c>
       <c r="D49" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -2055,13 +2073,13 @@
         <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>183</v>
+        <v>273</v>
       </c>
       <c r="D50" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2069,13 +2087,13 @@
         <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>184</v>
+        <v>274</v>
       </c>
       <c r="D51" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2083,13 +2101,13 @@
         <v>118</v>
       </c>
       <c r="C52" t="s">
-        <v>185</v>
+        <v>275</v>
       </c>
       <c r="D52" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2097,13 +2115,13 @@
         <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>186</v>
+        <v>276</v>
       </c>
       <c r="D53" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2111,13 +2129,13 @@
         <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>187</v>
+        <v>277</v>
       </c>
       <c r="D54" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>35</v>
       </c>
@@ -2125,13 +2143,13 @@
         <v>97</v>
       </c>
       <c r="C55" t="s">
-        <v>188</v>
+        <v>278</v>
       </c>
       <c r="D55" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2139,13 +2157,13 @@
         <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>189</v>
+        <v>279</v>
       </c>
       <c r="D56" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2153,13 +2171,13 @@
         <v>91</v>
       </c>
       <c r="C57" t="s">
-        <v>190</v>
+        <v>280</v>
       </c>
       <c r="D57" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -2167,13 +2185,13 @@
         <v>122</v>
       </c>
       <c r="C58" t="s">
-        <v>191</v>
+        <v>281</v>
       </c>
       <c r="D58" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2181,13 +2199,13 @@
         <v>123</v>
       </c>
       <c r="C59" t="s">
-        <v>192</v>
+        <v>282</v>
       </c>
       <c r="D59" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2195,13 +2213,13 @@
         <v>124</v>
       </c>
       <c r="C60" t="s">
-        <v>193</v>
+        <v>283</v>
       </c>
       <c r="D60" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -2209,13 +2227,13 @@
         <v>105</v>
       </c>
       <c r="C61" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="D61" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -2223,13 +2241,13 @@
         <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>195</v>
+        <v>286</v>
       </c>
       <c r="D62" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -2237,13 +2255,13 @@
         <v>125</v>
       </c>
       <c r="C63" t="s">
-        <v>196</v>
+        <v>287</v>
       </c>
       <c r="D63" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -2251,13 +2269,13 @@
         <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>197</v>
+        <v>289</v>
       </c>
       <c r="D64" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -2265,13 +2283,13 @@
         <v>95</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>290</v>
       </c>
       <c r="D65" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -2279,13 +2297,13 @@
         <v>95</v>
       </c>
       <c r="C66" t="s">
-        <v>199</v>
+        <v>291</v>
       </c>
       <c r="D66" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -2293,13 +2311,13 @@
         <v>121</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>292</v>
       </c>
       <c r="D67" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>64</v>
       </c>
@@ -2307,13 +2325,13 @@
         <v>126</v>
       </c>
       <c r="C68" t="s">
-        <v>201</v>
+        <v>293</v>
       </c>
       <c r="D68" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -2321,13 +2339,13 @@
         <v>123</v>
       </c>
       <c r="C69" t="s">
-        <v>202</v>
+        <v>294</v>
       </c>
       <c r="D69" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>66</v>
       </c>
@@ -2335,13 +2353,13 @@
         <v>110</v>
       </c>
       <c r="C70" t="s">
-        <v>203</v>
+        <v>295</v>
       </c>
       <c r="D70" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -2349,13 +2367,13 @@
         <v>95</v>
       </c>
       <c r="C71" t="s">
-        <v>204</v>
+        <v>296</v>
       </c>
       <c r="D71" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>32</v>
       </c>
@@ -2363,13 +2381,13 @@
         <v>127</v>
       </c>
       <c r="C72" t="s">
-        <v>205</v>
+        <v>297</v>
       </c>
       <c r="D72" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>68</v>
       </c>
@@ -2377,13 +2395,13 @@
         <v>87</v>
       </c>
       <c r="C73" t="s">
-        <v>206</v>
+        <v>298</v>
       </c>
       <c r="D73" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>69</v>
       </c>
@@ -2391,13 +2409,13 @@
         <v>85</v>
       </c>
       <c r="C74" t="s">
-        <v>207</v>
+        <v>299</v>
       </c>
       <c r="D74" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -2405,13 +2423,13 @@
         <v>128</v>
       </c>
       <c r="C75" t="s">
-        <v>208</v>
+        <v>300</v>
       </c>
       <c r="D75" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>71</v>
       </c>
@@ -2419,13 +2437,13 @@
         <v>87</v>
       </c>
       <c r="C76" t="s">
-        <v>209</v>
+        <v>301</v>
       </c>
       <c r="D76" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>72</v>
       </c>
@@ -2433,13 +2451,13 @@
         <v>89</v>
       </c>
       <c r="C77" t="s">
-        <v>210</v>
+        <v>302</v>
       </c>
       <c r="D77" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>73</v>
       </c>
@@ -2447,13 +2465,13 @@
         <v>129</v>
       </c>
       <c r="C78" t="s">
-        <v>211</v>
+        <v>303</v>
       </c>
       <c r="D78" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>45</v>
       </c>
@@ -2461,13 +2479,13 @@
         <v>117</v>
       </c>
       <c r="C79" t="s">
-        <v>212</v>
+        <v>304</v>
       </c>
       <c r="D79" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -2475,13 +2493,13 @@
         <v>124</v>
       </c>
       <c r="C80" t="s">
-        <v>213</v>
+        <v>305</v>
       </c>
       <c r="D80" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -2489,13 +2507,13 @@
         <v>124</v>
       </c>
       <c r="C81" t="s">
-        <v>214</v>
+        <v>306</v>
       </c>
       <c r="D81" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>22</v>
       </c>
@@ -2503,13 +2521,13 @@
         <v>115</v>
       </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>307</v>
       </c>
       <c r="D82" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -2517,13 +2535,13 @@
         <v>88</v>
       </c>
       <c r="C83" t="s">
-        <v>216</v>
+        <v>308</v>
       </c>
       <c r="D83" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>75</v>
       </c>
@@ -2531,13 +2549,13 @@
         <v>130</v>
       </c>
       <c r="C84" t="s">
-        <v>217</v>
+        <v>309</v>
       </c>
       <c r="D84" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -2545,13 +2563,13 @@
         <v>109</v>
       </c>
       <c r="C85" t="s">
-        <v>218</v>
+        <v>310</v>
       </c>
       <c r="D85" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>76</v>
       </c>
@@ -2559,13 +2577,13 @@
         <v>131</v>
       </c>
       <c r="C86" t="s">
-        <v>219</v>
+        <v>311</v>
       </c>
       <c r="D86" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>55</v>
       </c>
@@ -2573,13 +2591,13 @@
         <v>127</v>
       </c>
       <c r="C87" t="s">
-        <v>220</v>
+        <v>312</v>
       </c>
       <c r="D87" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>77</v>
       </c>
@@ -2587,13 +2605,13 @@
         <v>116</v>
       </c>
       <c r="C88" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
       <c r="D88" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>78</v>
       </c>
@@ -2601,13 +2619,13 @@
         <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>222</v>
+        <v>314</v>
       </c>
       <c r="D89" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>79</v>
       </c>
@@ -2615,13 +2633,13 @@
         <v>86</v>
       </c>
       <c r="C90" t="s">
-        <v>223</v>
+        <v>315</v>
       </c>
       <c r="D90" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>80</v>
       </c>
@@ -2629,13 +2647,13 @@
         <v>132</v>
       </c>
       <c r="C91" t="s">
-        <v>224</v>
+        <v>316</v>
       </c>
       <c r="D91" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2643,13 +2661,13 @@
         <v>133</v>
       </c>
       <c r="C92" t="s">
-        <v>225</v>
+        <v>317</v>
       </c>
       <c r="D92" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>32</v>
       </c>
@@ -2657,13 +2675,13 @@
         <v>98</v>
       </c>
       <c r="C93" t="s">
-        <v>226</v>
+        <v>318</v>
       </c>
       <c r="D93" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -2671,13 +2689,13 @@
         <v>134</v>
       </c>
       <c r="C94" t="s">
-        <v>227</v>
+        <v>319</v>
       </c>
       <c r="D94" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>31</v>
       </c>
@@ -2685,13 +2703,13 @@
         <v>86</v>
       </c>
       <c r="C95" t="s">
-        <v>228</v>
+        <v>320</v>
       </c>
       <c r="D95" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>56</v>
       </c>
@@ -2699,13 +2717,13 @@
         <v>125</v>
       </c>
       <c r="C96" t="s">
-        <v>229</v>
+        <v>321</v>
       </c>
       <c r="D96" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>65</v>
       </c>
@@ -2713,13 +2731,13 @@
         <v>134</v>
       </c>
       <c r="C97" t="s">
-        <v>230</v>
+        <v>322</v>
       </c>
       <c r="D97" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>82</v>
       </c>
@@ -2727,13 +2745,13 @@
         <v>85</v>
       </c>
       <c r="C98" t="s">
-        <v>231</v>
+        <v>323</v>
       </c>
       <c r="D98" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>76</v>
       </c>
@@ -2741,13 +2759,13 @@
         <v>104</v>
       </c>
       <c r="C99" t="s">
-        <v>232</v>
+        <v>324</v>
       </c>
       <c r="D99" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>83</v>
       </c>
@@ -2755,13 +2773,13 @@
         <v>99</v>
       </c>
       <c r="C100" t="s">
-        <v>233</v>
+        <v>325</v>
       </c>
       <c r="D100" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>84</v>
       </c>
@@ -2769,10 +2787,10 @@
         <v>123</v>
       </c>
       <c r="C101" t="s">
-        <v>234</v>
+        <v>327</v>
       </c>
       <c r="D101" t="s">
-        <v>327</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>